<commit_message>
-added OSA lab2 -finished Electro lab2
</commit_message>
<xml_diff>
--- a/ОСА/lab1/OSA_lab1.xlsx
+++ b/ОСА/lab1/OSA_lab1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="245" yWindow="109" windowWidth="14808" windowHeight="8015"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="46">
   <si>
     <t>I</t>
   </si>
@@ -151,25 +151,42 @@
     <t>3 эксперт</t>
   </si>
   <si>
-    <t>E=0,21q1+0,15q2+0,1q3+0,04q4+0,21q5+0,15q6+0,1q7+0,04q8</t>
-  </si>
-  <si>
-    <t>E=0,21q1+0,04q2+0,15q3+0,10q4+0,21q5+0,04q6+0,15q7+0,1q8</t>
-  </si>
-  <si>
-    <t>E=0,19q1+0,19q2+0,19q3+0,13q4+0,06q5+0,06q6+0,06q7+0,13q8</t>
+    <t>bi</t>
+  </si>
+  <si>
+    <t>Эксперт 1</t>
+  </si>
+  <si>
+    <t>Эксперт 2</t>
+  </si>
+  <si>
+    <t>Эксперт 3</t>
+  </si>
+  <si>
+    <t>0,20q1+0,13q2+0,15q3+0,11q4+0,20q5+0,13q6+0,15q7+0,11q8</t>
+  </si>
+  <si>
+    <t>i</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -233,6 +250,13 @@
       <family val="1"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -254,30 +278,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="3" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FF538DD5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -375,6 +399,19 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top/>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
@@ -382,7 +419,273 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top style="thin">
         <color rgb="FF3F3F3F"/>
@@ -390,68 +693,170 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="31" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Вывод" xfId="1" builtinId="21"/>
@@ -754,32 +1159,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R36"/>
+  <dimension ref="A1:AF37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+      <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="12" max="12" width="13" customWidth="1"/>
-    <col min="13" max="16" width="9.140625" customWidth="1"/>
+    <col min="13" max="16" width="9.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B1" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+    <row r="1" spans="1:32" ht="18.350000000000001" x14ac:dyDescent="0.3">
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
       <c r="K1" s="1"/>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="M1" s="4">
@@ -795,168 +1196,170 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
+    <row r="2" spans="1:32" ht="18.350000000000001" x14ac:dyDescent="0.3">
+      <c r="B2" s="58" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="60"/>
       <c r="K2" s="1"/>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="N2" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="O2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="P2" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="7" t="s">
+    <row r="3" spans="1:32" ht="18.350000000000001" x14ac:dyDescent="0.3">
+      <c r="B3" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="18">
         <v>1</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="18">
         <v>2</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="18">
         <v>3</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="18">
         <v>4</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="18">
         <v>5</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="18">
         <v>6</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="18">
         <v>7</v>
       </c>
-      <c r="J3" s="7">
+      <c r="J3" s="45">
         <v>8</v>
       </c>
       <c r="K3" s="1"/>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="5">
+      <c r="M3" s="16">
         <v>2</v>
       </c>
-      <c r="N3" s="5">
+      <c r="N3" s="16">
         <v>4</v>
       </c>
-      <c r="O3" s="5">
+      <c r="O3" s="16">
         <v>6</v>
       </c>
-      <c r="P3" s="5">
+      <c r="P3" s="16">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:32" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="47">
         <f>AVERAGE($M$1,$M$3)</f>
         <v>1.5</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="47">
         <f>AVERAGE($N$1,$N$3)</f>
         <v>3.5</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="47">
         <f>AVERAGE($O$1,$O$3)</f>
         <v>5.5</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="47">
         <f>AVERAGE($P$1,$P$3)</f>
         <v>7.5</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="47">
         <f>AVERAGE($M$1,$M$3)</f>
         <v>1.5</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="47">
         <f>AVERAGE($N$1,$N$3)</f>
         <v>3.5</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4" s="47">
         <f>AVERAGE($O$1,$O$3)</f>
         <v>5.5</v>
       </c>
-      <c r="J4" s="8">
+      <c r="J4" s="48">
         <f>AVERAGE($P$1,$P$3)</f>
         <v>7.5</v>
       </c>
       <c r="K4" s="2"/>
-      <c r="L4" s="6" t="s">
+      <c r="L4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="M4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="N4" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="6" t="s">
+      <c r="O4" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="P4" s="6" t="s">
+      <c r="P4" s="15" t="s">
         <v>14</v>
       </c>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
     </row>
-    <row r="5" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:32" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="49">
         <f>1-(C$4 - 1)/$J$3</f>
         <v>0.9375</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="49">
         <f t="shared" ref="D5:J5" si="0">1-(D$4 - 1)/$J$3</f>
         <v>0.6875</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="49">
         <f t="shared" si="0"/>
         <v>0.4375</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="49">
         <f t="shared" si="0"/>
         <v>0.1875</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="49">
         <f t="shared" si="0"/>
         <v>0.9375</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="49">
         <f t="shared" si="0"/>
         <v>0.6875</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5" s="49">
         <f t="shared" si="0"/>
         <v>0.4375</v>
       </c>
-      <c r="J5" s="9">
+      <c r="J5" s="50">
         <f t="shared" si="0"/>
         <v>0.1875</v>
       </c>
@@ -969,40 +1372,40 @@
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
     </row>
-    <row r="6" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:32" ht="19.05" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="49">
         <f>C$5/SUM($C$5:$J$5)</f>
         <v>0.20833333333333334</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="49">
         <f t="shared" ref="D6:J6" si="1">D$5/SUM($C$5:$J$5)</f>
         <v>0.15277777777777779</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="49">
         <f t="shared" si="1"/>
         <v>9.7222222222222224E-2</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="49">
         <f t="shared" si="1"/>
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="49">
         <f t="shared" si="1"/>
         <v>0.20833333333333334</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="49">
         <f t="shared" si="1"/>
         <v>0.15277777777777779</v>
       </c>
-      <c r="I6" s="9">
+      <c r="I6" s="49">
         <f t="shared" si="1"/>
         <v>9.7222222222222224E-2</v>
       </c>
-      <c r="J6" s="9">
+      <c r="J6" s="50">
         <f t="shared" si="1"/>
         <v>4.1666666666666664E-2</v>
       </c>
@@ -1014,20 +1417,37 @@
       <c r="P6" s="3"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
-    </row>
-    <row r="7" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="T6" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="U6" s="42"/>
+      <c r="V6" s="42"/>
+      <c r="W6" s="43"/>
+      <c r="X6" s="27"/>
+      <c r="Y6" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z6" s="26"/>
+      <c r="AA6" s="26"/>
+      <c r="AB6" s="26"/>
+      <c r="AC6" s="27"/>
+      <c r="AD6" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE6" s="26"/>
+      <c r="AF6" s="28"/>
+    </row>
+    <row r="7" spans="1:32" ht="19.05" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
-      <c r="B7" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="52"/>
       <c r="K7" s="2"/>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
@@ -1036,18 +1456,55 @@
       <c r="P7" s="3"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
-    </row>
-    <row r="8" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="T7" s="33">
+        <v>1</v>
+      </c>
+      <c r="U7" s="24">
+        <v>3</v>
+      </c>
+      <c r="V7" s="24">
+        <v>5</v>
+      </c>
+      <c r="W7" s="24">
+        <v>7</v>
+      </c>
+      <c r="X7" s="29"/>
+      <c r="Y7" s="19">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="20">
+        <v>3</v>
+      </c>
+      <c r="AA7" s="20">
+        <v>5</v>
+      </c>
+      <c r="AB7" s="20">
+        <v>7</v>
+      </c>
+      <c r="AC7" s="29"/>
+      <c r="AD7" s="19">
+        <v>1</v>
+      </c>
+      <c r="AE7" s="20">
+        <v>4</v>
+      </c>
+      <c r="AF7" s="30">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" ht="19.05" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
+      <c r="B8" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="59"/>
+      <c r="H8" s="59"/>
+      <c r="I8" s="59"/>
+      <c r="J8" s="60"/>
       <c r="K8" s="2"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
@@ -1056,18 +1513,71 @@
       <c r="P8" s="3"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
-    </row>
-    <row r="9" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="T8" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="U8" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="V8" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="W8" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="X8" s="29"/>
+      <c r="Y8" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z8" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA8" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB8" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC8" s="29"/>
+      <c r="AD8" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE8" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF8" s="32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" ht="19.05" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
+      <c r="B9" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="18">
+        <v>1</v>
+      </c>
+      <c r="D9" s="18">
+        <v>2</v>
+      </c>
+      <c r="E9" s="18">
+        <v>3</v>
+      </c>
+      <c r="F9" s="18">
+        <v>4</v>
+      </c>
+      <c r="G9" s="18">
+        <v>5</v>
+      </c>
+      <c r="H9" s="18">
+        <v>6</v>
+      </c>
+      <c r="I9" s="18">
+        <v>7</v>
+      </c>
+      <c r="J9" s="45">
+        <v>8</v>
+      </c>
       <c r="K9" s="2"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
@@ -1076,18 +1586,79 @@
       <c r="P9" s="3"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
-    </row>
-    <row r="10" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="T9" s="33">
+        <v>2</v>
+      </c>
+      <c r="U9" s="24">
+        <v>4</v>
+      </c>
+      <c r="V9" s="24">
+        <v>6</v>
+      </c>
+      <c r="W9" s="24">
+        <v>8</v>
+      </c>
+      <c r="X9" s="29"/>
+      <c r="Y9" s="23">
+        <v>2</v>
+      </c>
+      <c r="Z9" s="24">
+        <v>4</v>
+      </c>
+      <c r="AA9" s="24">
+        <v>6</v>
+      </c>
+      <c r="AB9" s="24">
+        <v>8</v>
+      </c>
+      <c r="AC9" s="29"/>
+      <c r="AD9" s="23">
+        <v>2</v>
+      </c>
+      <c r="AE9" s="24">
+        <v>5</v>
+      </c>
+      <c r="AF9" s="34">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" ht="19.05" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
+      <c r="B10" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="47">
+        <f>AVERAGE($M$11,$M$13)</f>
+        <v>1.5</v>
+      </c>
+      <c r="D10" s="47">
+        <f>AVERAGE($P$11,$P$13)</f>
+        <v>7.5</v>
+      </c>
+      <c r="E10" s="47">
+        <f>AVERAGE($N$11,$N$13)</f>
+        <v>3.5</v>
+      </c>
+      <c r="F10" s="47">
+        <f>AVERAGE($O$11,$O$13)</f>
+        <v>5.5</v>
+      </c>
+      <c r="G10" s="47">
+        <f>AVERAGE($M$11,$M$13)</f>
+        <v>1.5</v>
+      </c>
+      <c r="H10" s="47">
+        <f>AVERAGE($P$11,$P$13)</f>
+        <v>7.5</v>
+      </c>
+      <c r="I10" s="47">
+        <f>AVERAGE($N$11,$N$13)</f>
+        <v>3.5</v>
+      </c>
+      <c r="J10" s="48">
+        <f>AVERAGE($O$11,$O$13)</f>
+        <v>5.5</v>
+      </c>
       <c r="K10" s="2"/>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
@@ -1096,22 +1667,81 @@
       <c r="P10" s="3"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
-    </row>
-    <row r="11" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="T10" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="U10" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="V10" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="W10" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="X10" s="29"/>
+      <c r="Y10" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z10" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA10" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB10" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC10" s="29"/>
+      <c r="AD10" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE10" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF10" s="32" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" ht="19.05" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
-      <c r="B11" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
+      <c r="B11" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="49">
+        <f>1-(C$10 - 1)/$J$9</f>
+        <v>0.9375</v>
+      </c>
+      <c r="D11" s="49">
+        <f>1-(D$10 - 1)/$J$9</f>
+        <v>0.1875</v>
+      </c>
+      <c r="E11" s="49">
+        <f>1-(E$10 - 1)/$J$9</f>
+        <v>0.6875</v>
+      </c>
+      <c r="F11" s="49">
+        <f>1-(F$10 - 1)/$J$9</f>
+        <v>0.4375</v>
+      </c>
+      <c r="G11" s="49">
+        <f>1-(G$10 - 1)/$J$9</f>
+        <v>0.9375</v>
+      </c>
+      <c r="H11" s="49">
+        <f>1-(H$10 - 1)/$J$9</f>
+        <v>0.1875</v>
+      </c>
+      <c r="I11" s="49">
+        <f>1-(I$10 - 1)/$J$9</f>
+        <v>0.6875</v>
+      </c>
+      <c r="J11" s="50">
+        <f>1-(J$10 - 1)/$J$9</f>
+        <v>0.4375</v>
+      </c>
       <c r="K11" s="2"/>
-      <c r="L11" s="6" t="s">
+      <c r="L11" s="4" t="s">
         <v>6</v>
       </c>
       <c r="M11" s="4">
@@ -1128,177 +1758,187 @@
       </c>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
-    </row>
-    <row r="12" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="T11" s="35"/>
+      <c r="U11" s="29"/>
+      <c r="V11" s="29"/>
+      <c r="W11" s="29"/>
+      <c r="X11" s="29"/>
+      <c r="Y11" s="29"/>
+      <c r="Z11" s="29"/>
+      <c r="AA11" s="29"/>
+      <c r="AB11" s="29"/>
+      <c r="AC11" s="29"/>
+      <c r="AD11" s="23">
+        <v>3</v>
+      </c>
+      <c r="AE11" s="25"/>
+      <c r="AF11" s="34">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
+      <c r="B12" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="49">
+        <f>C$11/SUM($C$11:$J$11)</f>
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="D12" s="49">
+        <f>D$11/SUM($C$11:$J$11)</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E12" s="49">
+        <f>E$11/SUM($C$11:$J$11)</f>
+        <v>0.15277777777777779</v>
+      </c>
+      <c r="F12" s="49">
+        <f>F$11/SUM($C$11:$J$11)</f>
+        <v>9.7222222222222224E-2</v>
+      </c>
+      <c r="G12" s="49">
+        <f>G$11/SUM($C$11:$J$11)</f>
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="H12" s="49">
+        <f>H$11/SUM($C$11:$J$11)</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="I12" s="49">
+        <f>I$11/SUM($C$11:$J$11)</f>
+        <v>0.15277777777777779</v>
+      </c>
+      <c r="J12" s="50">
+        <f>J$11/SUM($C$11:$J$11)</f>
+        <v>9.7222222222222224E-2</v>
+      </c>
       <c r="K12" s="2"/>
-      <c r="L12" s="6" t="s">
+      <c r="L12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="M12" s="6" t="s">
+      <c r="M12" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="N12" s="6" t="s">
+      <c r="N12" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="O12" s="6" t="s">
+      <c r="O12" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="P12" s="6" t="s">
+      <c r="P12" s="15" t="s">
         <v>9</v>
       </c>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
-    </row>
-    <row r="13" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="T12" s="36"/>
+      <c r="U12" s="37"/>
+      <c r="V12" s="37"/>
+      <c r="W12" s="37"/>
+      <c r="X12" s="37"/>
+      <c r="Y12" s="37"/>
+      <c r="Z12" s="37"/>
+      <c r="AA12" s="37"/>
+      <c r="AB12" s="37"/>
+      <c r="AC12" s="37"/>
+      <c r="AD12" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE12" s="39"/>
+      <c r="AF12" s="40" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
-      <c r="B13" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="7">
-        <v>1</v>
-      </c>
-      <c r="D13" s="7">
+      <c r="B13" s="35"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="53"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="M13" s="16">
         <v>2</v>
       </c>
-      <c r="E13" s="7">
-        <v>3</v>
-      </c>
-      <c r="F13" s="7">
+      <c r="N13" s="16">
         <v>4</v>
       </c>
-      <c r="G13" s="7">
-        <v>5</v>
-      </c>
-      <c r="H13" s="7">
+      <c r="O13" s="16">
         <v>6</v>
       </c>
-      <c r="I13" s="7">
-        <v>7</v>
-      </c>
-      <c r="J13" s="7">
-        <v>8</v>
-      </c>
-      <c r="K13" s="2"/>
-      <c r="L13" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="M13" s="5">
-        <v>2</v>
-      </c>
-      <c r="N13" s="5">
-        <v>4</v>
-      </c>
-      <c r="O13" s="5">
-        <v>6</v>
-      </c>
-      <c r="P13" s="5">
+      <c r="P13" s="16">
         <v>8</v>
       </c>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
     </row>
-    <row r="14" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:32" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
-      <c r="B14" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="8">
-        <f>AVERAGE($M$11,$M$13)</f>
-        <v>1.5</v>
-      </c>
-      <c r="D14" s="8">
-        <f>AVERAGE($P$11,$P$13)</f>
-        <v>7.5</v>
-      </c>
-      <c r="E14" s="8">
-        <f>AVERAGE($N$11,$N$13)</f>
-        <v>3.5</v>
-      </c>
-      <c r="F14" s="8">
-        <f>AVERAGE($O$11,$O$13)</f>
-        <v>5.5</v>
-      </c>
-      <c r="G14" s="8">
-        <f>AVERAGE($M$11,$M$13)</f>
-        <v>1.5</v>
-      </c>
-      <c r="H14" s="8">
-        <f>AVERAGE($P$11,$P$13)</f>
-        <v>7.5</v>
-      </c>
-      <c r="I14" s="8">
-        <f>AVERAGE($N$11,$N$13)</f>
-        <v>3.5</v>
-      </c>
-      <c r="J14" s="8">
-        <f>AVERAGE($O$11,$O$13)</f>
-        <v>5.5</v>
-      </c>
+      <c r="B14" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="43"/>
       <c r="K14" s="2"/>
-      <c r="L14" s="6" t="s">
+      <c r="L14" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="M14" s="6" t="s">
+      <c r="M14" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="N14" s="6" t="s">
+      <c r="N14" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="O14" s="6" t="s">
+      <c r="O14" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="P14" s="6" t="s">
+      <c r="P14" s="15" t="s">
         <v>10</v>
       </c>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
     </row>
-    <row r="15" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:32" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="18">
+        <v>1</v>
+      </c>
+      <c r="D15" s="18">
         <v>2</v>
       </c>
-      <c r="C15" s="9">
-        <f>1-(C$14 - 1)/$J$13</f>
-        <v>0.9375</v>
-      </c>
-      <c r="D15" s="9">
-        <f t="shared" ref="D15:J15" si="2">1-(D$14 - 1)/$J$13</f>
-        <v>0.1875</v>
-      </c>
-      <c r="E15" s="9">
-        <f t="shared" si="2"/>
-        <v>0.6875</v>
-      </c>
-      <c r="F15" s="9">
-        <f t="shared" si="2"/>
-        <v>0.4375</v>
-      </c>
-      <c r="G15" s="9">
-        <f t="shared" si="2"/>
-        <v>0.9375</v>
-      </c>
-      <c r="H15" s="9">
-        <f t="shared" si="2"/>
-        <v>0.1875</v>
-      </c>
-      <c r="I15" s="9">
-        <f t="shared" si="2"/>
-        <v>0.6875</v>
-      </c>
-      <c r="J15" s="9">
-        <f t="shared" si="2"/>
-        <v>0.4375</v>
+      <c r="E15" s="18">
+        <v>3</v>
+      </c>
+      <c r="F15" s="18">
+        <v>4</v>
+      </c>
+      <c r="G15" s="18">
+        <v>5</v>
+      </c>
+      <c r="H15" s="18">
+        <v>6</v>
+      </c>
+      <c r="I15" s="18">
+        <v>7</v>
+      </c>
+      <c r="J15" s="45">
+        <v>8</v>
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="3"/>
@@ -1309,42 +1949,42 @@
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
     </row>
-    <row r="16" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:32" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
-      <c r="B16" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="9">
-        <f>C$15/SUM($C$15:$J$15)</f>
-        <v>0.20833333333333334</v>
-      </c>
-      <c r="D16" s="9">
-        <f t="shared" ref="D16:J16" si="3">D$15/SUM($C$15:$J$15)</f>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="E16" s="9">
-        <f t="shared" si="3"/>
-        <v>0.15277777777777779</v>
-      </c>
-      <c r="F16" s="9">
-        <f t="shared" si="3"/>
-        <v>9.7222222222222224E-2</v>
-      </c>
-      <c r="G16" s="9">
-        <f t="shared" si="3"/>
-        <v>0.20833333333333334</v>
-      </c>
-      <c r="H16" s="9">
-        <f t="shared" si="3"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="I16" s="9">
-        <f t="shared" si="3"/>
-        <v>0.15277777777777779</v>
-      </c>
-      <c r="J16" s="9">
-        <f t="shared" si="3"/>
-        <v>9.7222222222222224E-2</v>
+      <c r="B16" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="47">
+        <f>AVERAGE($M$21,$M$23,$M$25)</f>
+        <v>2</v>
+      </c>
+      <c r="D16" s="47">
+        <f>AVERAGE($M$21,$M$23,$M$25)</f>
+        <v>2</v>
+      </c>
+      <c r="E16" s="47">
+        <f>AVERAGE($M$21,$M$23,$M$25)</f>
+        <v>2</v>
+      </c>
+      <c r="F16" s="47">
+        <f>AVERAGE($N$21,$N$23)</f>
+        <v>4.5</v>
+      </c>
+      <c r="G16" s="47">
+        <f>AVERAGE($O$21,$O$23,$O$25)</f>
+        <v>7</v>
+      </c>
+      <c r="H16" s="47">
+        <f>AVERAGE($O$21,$O$23,$O$25)</f>
+        <v>7</v>
+      </c>
+      <c r="I16" s="47">
+        <f>AVERAGE($O$21,$O$23,$O$25)</f>
+        <v>7</v>
+      </c>
+      <c r="J16" s="48">
+        <f>AVERAGE($N$21,$N$23)</f>
+        <v>4.5</v>
       </c>
       <c r="K16" s="2"/>
       <c r="L16" s="3"/>
@@ -1355,19 +1995,43 @@
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
     </row>
-    <row r="17" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
-      <c r="B17" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="27"/>
+      <c r="B17" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="49">
+        <f>1-(C$16 - 1)/$J$15</f>
+        <v>0.875</v>
+      </c>
+      <c r="D17" s="49">
+        <f>1-(D$16 - 1)/$J$15</f>
+        <v>0.875</v>
+      </c>
+      <c r="E17" s="49">
+        <f>1-(E$16 - 1)/$J$15</f>
+        <v>0.875</v>
+      </c>
+      <c r="F17" s="49">
+        <f>1-(F$16 - 1)/$J$15</f>
+        <v>0.5625</v>
+      </c>
+      <c r="G17" s="49">
+        <f>1-(G$16 - 1)/$J$15</f>
+        <v>0.25</v>
+      </c>
+      <c r="H17" s="49">
+        <f>1-(H$16 - 1)/$J$15</f>
+        <v>0.25</v>
+      </c>
+      <c r="I17" s="49">
+        <f>1-(I$16 - 1)/$J$15</f>
+        <v>0.25</v>
+      </c>
+      <c r="J17" s="50">
+        <f>1-(J$16 - 1)/$J$15</f>
+        <v>0.5625</v>
+      </c>
       <c r="K17" s="2"/>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
@@ -1377,17 +2041,43 @@
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
     </row>
-    <row r="18" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
+      <c r="B18" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="49">
+        <f>C$17/SUM($C$17:$J$17)</f>
+        <v>0.19444444444444445</v>
+      </c>
+      <c r="D18" s="49">
+        <f>D$17/SUM($C$17:$J$17)</f>
+        <v>0.19444444444444445</v>
+      </c>
+      <c r="E18" s="49">
+        <f>E$17/SUM($C$17:$J$17)</f>
+        <v>0.19444444444444445</v>
+      </c>
+      <c r="F18" s="49">
+        <f>F$17/SUM($C$17:$J$17)</f>
+        <v>0.125</v>
+      </c>
+      <c r="G18" s="49">
+        <f>G$17/SUM($C$17:$J$17)</f>
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="H18" s="49">
+        <f>H$17/SUM($C$17:$J$17)</f>
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="I18" s="49">
+        <f>I$17/SUM($C$17:$J$17)</f>
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="J18" s="50">
+        <f>J$17/SUM($C$17:$J$17)</f>
+        <v>0.125</v>
+      </c>
       <c r="K18" s="2"/>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
@@ -1397,17 +2087,17 @@
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
     </row>
-    <row r="19" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="55"/>
+      <c r="F19" s="55"/>
+      <c r="G19" s="55"/>
+      <c r="H19" s="55"/>
+      <c r="I19" s="55"/>
+      <c r="J19" s="56"/>
       <c r="K19" s="2"/>
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
@@ -1417,17 +2107,43 @@
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
     </row>
-    <row r="20" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
+      <c r="B20" s="57" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="62">
+        <f>(1/$C$32)*(SUM(C$6,C$12,$C18))</f>
+        <v>0.20370370370370372</v>
+      </c>
+      <c r="D20" s="62">
+        <f>(1/$C$32)*(SUM(D$6,D$12,$C18))</f>
+        <v>0.12962962962962962</v>
+      </c>
+      <c r="E20" s="62">
+        <f>(1/$C$32)*(SUM(E$6,E$12,$C18))</f>
+        <v>0.14814814814814814</v>
+      </c>
+      <c r="F20" s="62">
+        <f>(1/$C$32)*(SUM(F$6,F$12,$C18))</f>
+        <v>0.11111111111111112</v>
+      </c>
+      <c r="G20" s="62">
+        <f>(1/$C$32)*(SUM(G$6,G$12,$C18))</f>
+        <v>0.20370370370370372</v>
+      </c>
+      <c r="H20" s="62">
+        <f>(1/$C$32)*(SUM(H$6,H$12,$C18))</f>
+        <v>0.12962962962962962</v>
+      </c>
+      <c r="I20" s="62">
+        <f>(1/$C$32)*(SUM(I$6,I$12,$C18))</f>
+        <v>0.14814814814814814</v>
+      </c>
+      <c r="J20" s="63">
+        <f>(1/$C$32)*(SUM(J$6,J$12,$C18))</f>
+        <v>0.11111111111111112</v>
+      </c>
       <c r="K20" s="2"/>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
@@ -1437,21 +2153,10 @@
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
     </row>
-    <row r="21" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
-      <c r="B21" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="23"/>
       <c r="K21" s="2"/>
-      <c r="L21" s="6" t="s">
+      <c r="L21" s="4" t="s">
         <v>6</v>
       </c>
       <c r="M21" s="4">
@@ -1467,173 +2172,70 @@
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
     </row>
-    <row r="22" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="24"/>
-      <c r="J22" s="24"/>
+      <c r="C22" t="s">
+        <v>44</v>
+      </c>
       <c r="K22" s="2"/>
-      <c r="L22" s="6" t="s">
+      <c r="L22" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="M22" s="6" t="s">
+      <c r="M22" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="N22" s="6" t="s">
+      <c r="N22" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="O22" s="6" t="s">
+      <c r="O22" s="15" t="s">
         <v>8</v>
       </c>
       <c r="P22" s="3"/>
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
     </row>
-    <row r="23" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
-      <c r="B23" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C23" s="7">
-        <v>1</v>
-      </c>
-      <c r="D23" s="7">
+      <c r="K23" s="2"/>
+      <c r="L23" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="M23" s="16">
         <v>2</v>
       </c>
-      <c r="E23" s="7">
-        <v>3</v>
-      </c>
-      <c r="F23" s="7">
-        <v>4</v>
-      </c>
-      <c r="G23" s="7">
+      <c r="N23" s="16">
         <v>5</v>
       </c>
-      <c r="H23" s="7">
-        <v>6</v>
-      </c>
-      <c r="I23" s="7">
-        <v>7</v>
-      </c>
-      <c r="J23" s="7">
-        <v>8</v>
-      </c>
-      <c r="K23" s="2"/>
-      <c r="L23" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="M23" s="5">
-        <v>2</v>
-      </c>
-      <c r="N23" s="5">
-        <v>5</v>
-      </c>
-      <c r="O23" s="5">
+      <c r="O23" s="16">
         <v>7</v>
       </c>
       <c r="P23" s="3"/>
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
     </row>
-    <row r="24" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
-      <c r="B24" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24" s="8">
-        <f>AVERAGE($M$21,$M$23,$M$25)</f>
-        <v>2</v>
-      </c>
-      <c r="D24" s="8">
-        <f>AVERAGE($M$21,$M$23,$M$25)</f>
-        <v>2</v>
-      </c>
-      <c r="E24" s="8">
-        <f>AVERAGE($M$21,$M$23,$M$25)</f>
-        <v>2</v>
-      </c>
-      <c r="F24" s="8">
-        <f>AVERAGE($N$21,$N$23)</f>
-        <v>4.5</v>
-      </c>
-      <c r="G24" s="8">
-        <f>AVERAGE($O$21,$O$23,$O$25)</f>
-        <v>7</v>
-      </c>
-      <c r="H24" s="8">
-        <f>AVERAGE($O$21,$O$23,$O$25)</f>
-        <v>7</v>
-      </c>
-      <c r="I24" s="8">
-        <f>AVERAGE($O$21,$O$23,$O$25)</f>
-        <v>7</v>
-      </c>
-      <c r="J24" s="8">
-        <f>AVERAGE($N$21,$N$23)</f>
-        <v>4.5</v>
-      </c>
       <c r="K24" s="2"/>
-      <c r="L24" s="6" t="s">
+      <c r="L24" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="M24" s="6" t="s">
+      <c r="M24" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="N24" s="6" t="s">
+      <c r="N24" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="O24" s="6" t="s">
+      <c r="O24" s="15" t="s">
         <v>10</v>
       </c>
       <c r="P24" s="3"/>
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
     </row>
-    <row r="25" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
-      <c r="B25" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C25" s="9">
-        <f>1-(C$24 - 1)/$J$23</f>
-        <v>0.875</v>
-      </c>
-      <c r="D25" s="9">
-        <f t="shared" ref="D25:J25" si="4">1-(D$24 - 1)/$J$23</f>
-        <v>0.875</v>
-      </c>
-      <c r="E25" s="9">
-        <f t="shared" si="4"/>
-        <v>0.875</v>
-      </c>
-      <c r="F25" s="9">
-        <f t="shared" si="4"/>
-        <v>0.5625</v>
-      </c>
-      <c r="G25" s="9">
-        <f t="shared" si="4"/>
-        <v>0.25</v>
-      </c>
-      <c r="H25" s="9">
-        <f t="shared" si="4"/>
-        <v>0.25</v>
-      </c>
-      <c r="I25" s="9">
-        <f t="shared" si="4"/>
-        <v>0.25</v>
-      </c>
-      <c r="J25" s="9">
-        <f t="shared" si="4"/>
-        <v>0.5625</v>
-      </c>
       <c r="K25" s="2"/>
-      <c r="L25" s="6" t="s">
+      <c r="L25" s="4" t="s">
         <v>6</v>
       </c>
       <c r="M25" s="4">
@@ -1647,72 +2249,24 @@
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
     </row>
-    <row r="26" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
-      <c r="B26" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" s="9">
-        <f>C$25/SUM($C$25:$J$25)</f>
-        <v>0.19444444444444445</v>
-      </c>
-      <c r="D26" s="9">
-        <f t="shared" ref="D26:J26" si="5">D$25/SUM($C$25:$J$25)</f>
-        <v>0.19444444444444445</v>
-      </c>
-      <c r="E26" s="9">
-        <f t="shared" si="5"/>
-        <v>0.19444444444444445</v>
-      </c>
-      <c r="F26" s="9">
-        <f t="shared" si="5"/>
-        <v>0.125</v>
-      </c>
-      <c r="G26" s="9">
-        <f t="shared" si="5"/>
-        <v>5.5555555555555552E-2</v>
-      </c>
-      <c r="H26" s="9">
-        <f t="shared" si="5"/>
-        <v>5.5555555555555552E-2</v>
-      </c>
-      <c r="I26" s="9">
-        <f t="shared" si="5"/>
-        <v>5.5555555555555552E-2</v>
-      </c>
-      <c r="J26" s="9">
-        <f t="shared" si="5"/>
-        <v>0.125</v>
-      </c>
-      <c r="K26" s="2"/>
-      <c r="L26" s="6" t="s">
+      <c r="L26" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="M26" s="6" t="s">
+      <c r="M26" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="N26" s="6"/>
-      <c r="O26" s="6" t="s">
+      <c r="N26" s="17"/>
+      <c r="O26" s="15" t="s">
         <v>12</v>
       </c>
       <c r="P26" s="3"/>
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
     </row>
-    <row r="27" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
-      <c r="B27" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="27"/>
-      <c r="I27" s="27"/>
-      <c r="J27" s="27"/>
-      <c r="K27" s="2"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -1721,7 +2275,7 @@
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
     </row>
-    <row r="28" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1741,17 +2295,8 @@
       <c r="Q28" s="2"/>
       <c r="R28" s="2"/>
     </row>
-    <row r="29" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
@@ -1761,177 +2306,170 @@
       <c r="Q29" s="2"/>
       <c r="R29" s="2"/>
     </row>
-    <row r="30" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="1"/>
-      <c r="C30" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="H30" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="I30" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="J30" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="K30" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="L30" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="M30" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="N30" s="26" t="s">
-        <v>13</v>
-      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
       <c r="O30" s="2"/>
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
     </row>
-    <row r="31" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="1"/>
-      <c r="C31" s="2">
-        <v>3</v>
-      </c>
-      <c r="D31" s="2">
-        <v>8</v>
+      <c r="C31" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
-      <c r="G31" s="10">
-        <f>M1+M11+M21</f>
-        <v>3</v>
-      </c>
-      <c r="H31" s="10">
-        <f>N1+P13+M23</f>
+      <c r="G31" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H31" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I31" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J31" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="K31" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="L31" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="M31" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="N31" s="12" t="s">
         <v>13</v>
-      </c>
-      <c r="I31" s="10">
-        <f>O1+N11+M25</f>
-        <v>11</v>
-      </c>
-      <c r="J31" s="10">
-        <f>P3+O11+N21</f>
-        <v>17</v>
-      </c>
-      <c r="K31" s="10">
-        <f>M3+M13+O21</f>
-        <v>10</v>
-      </c>
-      <c r="L31" s="10">
-        <f>N3+P13+O23</f>
-        <v>19</v>
-      </c>
-      <c r="M31" s="10">
-        <f>O3+N13+O25</f>
-        <v>18</v>
-      </c>
-      <c r="N31" s="11">
-        <f>P1+O13+N23</f>
-        <v>18</v>
       </c>
       <c r="O31" s="2"/>
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
     </row>
-    <row r="32" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="1"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
+      <c r="C32" s="2">
+        <v>3</v>
+      </c>
+      <c r="D32" s="2">
+        <v>8</v>
+      </c>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
-      <c r="G32" s="12">
-        <f>(G$31-(0.5*$C$31*(D31+1)))^2</f>
-        <v>110.25</v>
-      </c>
-      <c r="H32" s="12">
-        <f t="shared" ref="H32:N32" si="6">((H$31)-(0.5*$C$31*($D$31+1)))^2</f>
-        <v>0.25</v>
-      </c>
-      <c r="I32" s="12">
-        <f t="shared" si="6"/>
-        <v>6.25</v>
-      </c>
-      <c r="J32" s="12">
-        <f t="shared" si="6"/>
-        <v>12.25</v>
-      </c>
-      <c r="K32" s="12">
-        <f t="shared" si="6"/>
-        <v>12.25</v>
-      </c>
-      <c r="L32" s="12">
-        <f t="shared" si="6"/>
-        <v>30.25</v>
-      </c>
-      <c r="M32" s="12">
-        <f t="shared" si="6"/>
-        <v>20.25</v>
-      </c>
-      <c r="N32" s="13">
-        <f t="shared" si="6"/>
-        <v>20.25</v>
+      <c r="G32" s="5">
+        <f>M1+M11+M21</f>
+        <v>3</v>
+      </c>
+      <c r="H32" s="5">
+        <f>N1+P13+M23</f>
+        <v>13</v>
+      </c>
+      <c r="I32" s="5">
+        <f>O1+N11+M25</f>
+        <v>11</v>
+      </c>
+      <c r="J32" s="5">
+        <f>P3+O11+N21</f>
+        <v>17</v>
+      </c>
+      <c r="K32" s="5">
+        <f>M3+M13+O21</f>
+        <v>10</v>
+      </c>
+      <c r="L32" s="5">
+        <f>N3+P13+O23</f>
+        <v>19</v>
+      </c>
+      <c r="M32" s="5">
+        <f>O3+N13+O25</f>
+        <v>18</v>
+      </c>
+      <c r="N32" s="6">
+        <f>P1+O13+N23</f>
+        <v>18</v>
       </c>
       <c r="O32" s="2"/>
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
     </row>
-    <row r="33" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:18" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
       <c r="B33" s="1"/>
-      <c r="C33" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D33" s="2">
-        <f>SUM($G$32:$N$32)</f>
-        <v>212</v>
-      </c>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
+      <c r="G33" s="7">
+        <f>(G$32-(0.5*$C$32*(D32+1)))^2</f>
+        <v>110.25</v>
+      </c>
+      <c r="H33" s="7">
+        <f t="shared" ref="H33:N33" si="2">((H$32)-(0.5*$C$32*($D$32+1)))^2</f>
+        <v>0.25</v>
+      </c>
+      <c r="I33" s="7">
+        <f t="shared" si="2"/>
+        <v>6.25</v>
+      </c>
+      <c r="J33" s="7">
+        <f t="shared" si="2"/>
+        <v>12.25</v>
+      </c>
+      <c r="K33" s="7">
+        <f t="shared" si="2"/>
+        <v>12.25</v>
+      </c>
+      <c r="L33" s="7">
+        <f t="shared" si="2"/>
+        <v>30.25</v>
+      </c>
+      <c r="M33" s="7">
+        <f t="shared" si="2"/>
+        <v>20.25</v>
+      </c>
+      <c r="N33" s="8">
+        <f t="shared" si="2"/>
+        <v>20.25</v>
+      </c>
       <c r="O33" s="2"/>
       <c r="P33" s="2"/>
       <c r="Q33" s="2"/>
       <c r="R33" s="2"/>
     </row>
-    <row r="34" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
+      <c r="B34" s="1"/>
       <c r="C34" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D34" s="2">
-        <f>(12*D33)/(($C$31^2)*(($D$31^3)-$D$31))</f>
-        <v>0.56084656084656082</v>
-      </c>
-      <c r="E34" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="F34" s="14"/>
+        <f>SUM($G$33:$N$33)</f>
+        <v>212</v>
+      </c>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
@@ -1945,13 +2483,20 @@
       <c r="Q34" s="2"/>
       <c r="R34" s="2"/>
     </row>
-    <row r="35" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:18" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
+      <c r="C35" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" s="2">
+        <f>(12*D34)/(($C$32^2)*(($D$32^3)-$D$32))</f>
+        <v>0.56084656084656082</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F35" s="13"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
@@ -1965,7 +2510,7 @@
       <c r="Q35" s="2"/>
       <c r="R35" s="2"/>
     </row>
-    <row r="36" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:18" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -1985,15 +2530,36 @@
       <c r="Q36" s="2"/>
       <c r="R36" s="2"/>
     </row>
+    <row r="37" spans="1:18" ht="18.350000000000001" x14ac:dyDescent="0.3">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="2"/>
+      <c r="R37" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="B1:J2"/>
-    <mergeCell ref="B11:J12"/>
-    <mergeCell ref="B21:J22"/>
+  <mergeCells count="8">
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="T6:W6"/>
+    <mergeCell ref="Y6:AB6"/>
+    <mergeCell ref="AD6:AF6"/>
+    <mergeCell ref="B8:J8"/>
+    <mergeCell ref="B14:J14"/>
+    <mergeCell ref="E35:F35"/>
     <mergeCell ref="B7:J7"/>
-    <mergeCell ref="B17:J17"/>
-    <mergeCell ref="B27:J27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2005,10 +2571,10 @@
   <dimension ref="A2:M17"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -2026,7 +2592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -2041,343 +2607,343 @@
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
     </row>
-    <row r="6" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
-      <c r="B6" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="20">
+      <c r="B6" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="10">
         <v>1</v>
       </c>
-      <c r="D6" s="20">
+      <c r="D6" s="10">
         <v>2</v>
       </c>
-      <c r="E6" s="20">
+      <c r="E6" s="10">
         <v>3</v>
       </c>
-      <c r="F6" s="20">
+      <c r="F6" s="10">
         <v>4</v>
       </c>
-      <c r="G6" s="20">
+      <c r="G6" s="10">
         <v>5</v>
       </c>
-      <c r="H6" s="20">
+      <c r="H6" s="10">
         <v>6</v>
       </c>
-      <c r="I6" s="20">
+      <c r="I6" s="10">
         <v>7</v>
       </c>
-      <c r="J6" s="20">
+      <c r="J6" s="10">
         <v>8</v>
       </c>
-      <c r="K6" s="21" t="s">
+      <c r="K6" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="L6" s="21"/>
+      <c r="L6" s="70"/>
       <c r="M6" s="2"/>
     </row>
-    <row r="7" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="9">
         <v>1</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="9">
         <v>0.9</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="9">
         <v>0.7</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="9">
         <v>0.6</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="9">
         <v>0.5</v>
       </c>
-      <c r="H7" s="16">
+      <c r="H7" s="65">
         <v>0.4</v>
       </c>
-      <c r="I7" s="17">
+      <c r="I7" s="66">
         <v>0.3</v>
       </c>
-      <c r="J7" s="17">
+      <c r="J7" s="66">
         <v>0.2</v>
       </c>
-      <c r="K7" s="15" t="s">
+      <c r="K7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="L7" s="15" t="s">
+      <c r="L7" s="9" t="s">
         <v>23</v>
       </c>
       <c r="M7" s="2"/>
     </row>
-    <row r="8" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="9">
         <v>1</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="9">
         <v>0.9</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="9">
         <v>0.7</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="9">
         <v>0.6</v>
       </c>
-      <c r="G8" s="16">
+      <c r="G8" s="65">
         <v>0.5</v>
       </c>
-      <c r="H8" s="17">
+      <c r="H8" s="66">
         <v>0.4</v>
       </c>
-      <c r="I8" s="17">
+      <c r="I8" s="66">
         <v>0.3</v>
       </c>
-      <c r="J8" s="17">
+      <c r="J8" s="66">
         <v>0.2</v>
       </c>
-      <c r="K8" s="15" t="s">
+      <c r="K8" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="L8" s="15" t="s">
+      <c r="L8" s="9" t="s">
         <v>26</v>
       </c>
       <c r="M8" s="2"/>
     </row>
-    <row r="9" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="9">
         <v>1</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="9">
         <v>0.9</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="9">
         <v>0.7</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="65">
         <v>0.6</v>
       </c>
-      <c r="G9" s="17">
+      <c r="G9" s="66">
         <v>0.5</v>
       </c>
-      <c r="H9" s="17">
+      <c r="H9" s="66">
         <v>0.4</v>
       </c>
-      <c r="I9" s="17">
+      <c r="I9" s="66">
         <v>0.3</v>
       </c>
-      <c r="J9" s="17">
+      <c r="J9" s="66">
         <v>0.2</v>
       </c>
-      <c r="K9" s="15" t="s">
+      <c r="K9" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="L9" s="15" t="s">
+      <c r="L9" s="9" t="s">
         <v>24</v>
       </c>
       <c r="M9" s="2"/>
     </row>
-    <row r="10" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="9">
         <v>2</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="9">
         <v>1.9</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="65">
         <v>1.7</v>
       </c>
-      <c r="F10" s="17">
+      <c r="F10" s="66">
         <v>1.6</v>
       </c>
-      <c r="G10" s="17">
+      <c r="G10" s="66">
         <v>0.5</v>
       </c>
-      <c r="H10" s="17">
+      <c r="H10" s="66">
         <v>0.4</v>
       </c>
-      <c r="I10" s="17">
+      <c r="I10" s="66">
         <v>0.3</v>
       </c>
-      <c r="J10" s="17">
+      <c r="J10" s="66">
         <v>0.2</v>
       </c>
-      <c r="K10" s="15" t="s">
+      <c r="K10" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="L10" s="15" t="s">
+      <c r="L10" s="9" t="s">
         <v>25</v>
       </c>
       <c r="M10" s="2"/>
     </row>
-    <row r="11" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="9">
         <v>3</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="65">
         <v>2.9</v>
       </c>
-      <c r="E11" s="17">
+      <c r="E11" s="66">
         <v>2.7</v>
       </c>
-      <c r="F11" s="17">
+      <c r="F11" s="66">
         <v>1.6</v>
       </c>
-      <c r="G11" s="17">
+      <c r="G11" s="66">
         <v>0.5</v>
       </c>
-      <c r="H11" s="17">
+      <c r="H11" s="66">
         <v>0.4</v>
       </c>
-      <c r="I11" s="17">
+      <c r="I11" s="66">
         <v>0.3</v>
       </c>
-      <c r="J11" s="17">
+      <c r="J11" s="66">
         <v>0.2</v>
       </c>
-      <c r="K11" s="15" t="s">
+      <c r="K11" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="L11" s="15" t="s">
+      <c r="L11" s="9" t="s">
         <v>27</v>
       </c>
       <c r="M11" s="2"/>
     </row>
-    <row r="12" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12" s="65">
         <v>3</v>
       </c>
-      <c r="D12" s="17">
+      <c r="D12" s="66">
         <v>2.9</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12" s="66">
         <v>2.7</v>
       </c>
-      <c r="F12" s="17">
+      <c r="F12" s="66">
         <v>1.6</v>
       </c>
-      <c r="G12" s="17">
+      <c r="G12" s="66">
         <v>0.5</v>
       </c>
-      <c r="H12" s="17">
+      <c r="H12" s="66">
         <v>0.4</v>
       </c>
-      <c r="I12" s="17">
+      <c r="I12" s="66">
         <v>0.3</v>
       </c>
-      <c r="J12" s="17">
+      <c r="J12" s="66">
         <v>0.2</v>
       </c>
-      <c r="K12" s="15" t="s">
+      <c r="K12" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="L12" s="15" t="s">
+      <c r="L12" s="9" t="s">
         <v>35</v>
       </c>
       <c r="M12" s="2"/>
     </row>
-    <row r="13" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C13" s="64">
         <v>3</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="64">
         <v>2.9</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E13" s="64">
         <v>2.7</v>
       </c>
-      <c r="F13" s="18">
+      <c r="F13" s="64">
         <v>1.6</v>
       </c>
-      <c r="G13" s="18">
+      <c r="G13" s="64">
         <v>0.5</v>
       </c>
-      <c r="H13" s="18">
+      <c r="H13" s="64">
         <v>0.4</v>
       </c>
-      <c r="I13" s="18">
+      <c r="I13" s="64">
         <v>0.3</v>
       </c>
-      <c r="J13" s="18">
+      <c r="J13" s="64">
         <v>0.2</v>
       </c>
-      <c r="K13" s="15" t="s">
+      <c r="K13" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="L13" s="15">
+      <c r="L13" s="9">
         <f>SUM($C$13:$J$13)</f>
         <v>11.600000000000001</v>
       </c>
       <c r="M13" s="2"/>
     </row>
-    <row r="14" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="67" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="19">
+      <c r="C14" s="68">
         <f>C$13/$L$13</f>
         <v>0.25862068965517238</v>
       </c>
-      <c r="D14" s="19">
+      <c r="D14" s="68">
         <f t="shared" ref="D14:J14" si="0">D$13/$L$13</f>
         <v>0.24999999999999997</v>
       </c>
-      <c r="E14" s="19">
+      <c r="E14" s="68">
         <f t="shared" si="0"/>
         <v>0.23275862068965517</v>
       </c>
-      <c r="F14" s="19">
+      <c r="F14" s="68">
         <f t="shared" si="0"/>
         <v>0.13793103448275862</v>
       </c>
-      <c r="G14" s="19">
+      <c r="G14" s="68">
         <f t="shared" si="0"/>
         <v>4.3103448275862065E-2</v>
       </c>
-      <c r="H14" s="19">
+      <c r="H14" s="68">
         <f t="shared" si="0"/>
         <v>3.4482758620689655E-2</v>
       </c>
-      <c r="I14" s="19">
+      <c r="I14" s="68">
         <f t="shared" si="0"/>
         <v>2.5862068965517238E-2</v>
       </c>
-      <c r="J14" s="19">
+      <c r="J14" s="68">
         <f t="shared" si="0"/>
         <v>1.7241379310344827E-2</v>
       </c>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
       <c r="M14" s="2"/>
     </row>
-    <row r="15" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -2392,7 +2958,7 @@
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
     </row>
-    <row r="16" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -2407,7 +2973,7 @@
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
     </row>
-    <row r="17" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -2423,9 +2989,6 @@
       <c r="M17" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="K6:L6"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -2437,7 +3000,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>